<commit_message>
# PT-35 - Analisis de riesgos iniciales
</commit_message>
<xml_diff>
--- a/docs/Planilla Registro de Riesgos.xlsx
+++ b/docs/Planilla Registro de Riesgos.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facu\Materias Actuales\75.47 - Taller de Desarrollo de Proyectos II\Repositorio\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Planificación" sheetId="3" r:id="rId3"/>
     <sheet name="Estado" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>#</t>
   </si>
@@ -89,24 +84,12 @@
     <t>Requerimientos</t>
   </si>
   <si>
-    <t>Dado que un miembro del equipo podría renunciar, se produciría una falta de personal adecuado.</t>
-  </si>
-  <si>
-    <t>Recursos</t>
-  </si>
-  <si>
     <t>1) Mala captura de requisitos.      2) Mal análisis de requisitos.</t>
   </si>
   <si>
     <t>1) Retraso de cronograma.           2) Problemas con el cliente.</t>
   </si>
   <si>
-    <t>1) Insatisfacción.                                2) Problemas personales.</t>
-  </si>
-  <si>
-    <t>1) Escasez de personal.                  2) Mayor esfuerzo del equipo para cubrir la ausencia.</t>
-  </si>
-  <si>
     <t>Dado que podrían existir cambios constantes de requerimientos, se retrasaría la entrega del producto final.</t>
   </si>
   <si>
@@ -120,6 +103,39 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Ambiente</t>
+  </si>
+  <si>
+    <t>1) No se vera si se superan los contratiempos generales, al ser una demo de tipo local</t>
+  </si>
+  <si>
+    <t>1) Entrega demorada del producto final</t>
+  </si>
+  <si>
+    <t>Plan de Mitigacion</t>
+  </si>
+  <si>
+    <t>Dado que las fechas de exámenes se podrían acumular en un periodo corto de tiempo, se dedicaría una menor cantidad de horas al proyecto en dicho periodo</t>
+  </si>
+  <si>
+    <t>1) Los integrantes del equipo son estudiantes.                                          2) Los exámenes se toman dentro de un periodo acotado</t>
+  </si>
+  <si>
+    <t>1) Menor producción durante el periodo</t>
+  </si>
+  <si>
+    <t>Si no hubiese internet donde se realiza la entrega de funcionalidad, la realización de las demos serian menos cercanas a la realidad.</t>
+  </si>
+  <si>
+    <t>1) El ambiente de entrega posee complicaciones con internet inalámbrico</t>
+  </si>
+  <si>
+    <t>Si se desarrollase el servicio de compra por tarjeta de crédito, podrían existir complicaciones con la tecnología del servicio que retrase el cronograma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Tecnología nueva                           </t>
   </si>
 </sst>
 </file>
@@ -312,31 +328,136 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -349,9 +470,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -364,130 +483,25 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -516,11 +530,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -557,63 +617,28 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -888,7 +913,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -896,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:H23"/>
+  <dimension ref="D2:H24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:H7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,13 +954,13 @@
   <sheetData>
     <row r="2" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="33"/>
     </row>
     <row r="4" spans="4:8" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="3" t="s">
@@ -955,71 +980,92 @@
       </c>
     </row>
     <row r="5" spans="4:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D5" s="27">
+      <c r="D5" s="12">
         <v>1</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="D6" s="16">
+        <v>2</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D7" s="16">
+        <v>3</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="D8" s="16">
+        <v>4</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="F8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="4:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="D6" s="31">
-        <v>2</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="8" t="s">
+      <c r="H8" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="4:8" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="33">
-        <v>3</v>
-      </c>
-      <c r="E7" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="35" t="s">
+    </row>
+    <row r="9" spans="4:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="18">
+        <v>5</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="36" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D8" s="2"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D9" s="2"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
+      <c r="G9" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D10" s="2"/>
       <c r="E10" s="1"/>
       <c r="F10" s="7"/>
       <c r="G10" s="1"/>
@@ -1051,7 +1097,7 @@
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.25">
       <c r="E15" s="1"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
@@ -1074,6 +1120,7 @@
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
       <c r="F19" s="2"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1084,6 +1131,7 @@
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="F21" s="2"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
@@ -1094,22 +1142,26 @@
     <row r="23" spans="5:8" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,70 +1174,100 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="18"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="45" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="27">
+      <c r="B5" s="12">
         <v>1</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="22">
         <v>0.2</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="E5" s="23">
+        <f>C5*D5</f>
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>2</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="E6" s="24">
+        <f t="shared" ref="E6:E9" si="0">C6*D6</f>
+        <v>0.55999999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>3</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.9</v>
+      </c>
+      <c r="D7" s="10">
         <v>0.5</v>
       </c>
-      <c r="E5" s="38">
-        <f>C5*D5</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="31">
-        <v>2</v>
-      </c>
-      <c r="C6" s="11">
+      <c r="E7" s="24">
+        <f t="shared" si="0"/>
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="E8" s="24">
+        <f t="shared" si="0"/>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18">
+        <v>5</v>
+      </c>
+      <c r="C9" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="25">
         <v>0.4</v>
       </c>
-      <c r="D6" s="11">
-        <v>0.6</v>
-      </c>
-      <c r="E6" s="42">
-        <f>C6*D6</f>
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33">
-        <v>3</v>
-      </c>
-      <c r="C7" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="40">
-        <v>0.6</v>
-      </c>
-      <c r="E7" s="43">
-        <f>C7*D7</f>
-        <v>0.3</v>
+      <c r="E9" s="26">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -1198,71 +1280,97 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E7"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="19" t="s">
+    <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="39"/>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="F4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="27">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="12">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="31">
+      <c r="C5" s="49"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
         <v>2</v>
       </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="39"/>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33">
+      <c r="C6" s="46"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="24"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
         <v>3</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="24"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="24"/>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18">
+        <v>5</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1270,10 +1378,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1287,74 +1395,104 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="24"/>
-    </row>
-    <row r="4" spans="2:6" s="26" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="3" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="42"/>
+    </row>
+    <row r="4" spans="2:6" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="45" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="27">
+      <c r="B5" s="12">
         <v>1</v>
       </c>
-      <c r="C5" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="37"/>
-      <c r="E5" s="44">
-        <v>41524</v>
-      </c>
-      <c r="F5" s="45" t="s">
-        <v>30</v>
+      <c r="C5" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="27">
+        <v>41531</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="31">
+      <c r="B6" s="16">
         <v>2</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="11"/>
-      <c r="E6" s="25">
-        <v>41524</v>
-      </c>
-      <c r="F6" s="46" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="33">
+      <c r="C6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="10"/>
+      <c r="E6" s="47">
+        <v>41531</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
         <v>3</v>
       </c>
-      <c r="C7" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" s="40"/>
-      <c r="E7" s="48">
-        <v>41524</v>
-      </c>
-      <c r="F7" s="49" t="s">
-        <v>30</v>
+      <c r="C7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="47">
+        <v>41531</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="16">
+        <v>4</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="47">
+        <v>41531</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18">
+        <v>5</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="25"/>
+      <c r="E9" s="50">
+        <v>41531</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[PT-86 Riesgos - Planes de Mitigación/Contingencia/Respuesta/Umbrales] Completed
</commit_message>
<xml_diff>
--- a/docs/Planilla Registro de Riesgos.xlsx
+++ b/docs/Planilla Registro de Riesgos.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facu\Materias Actuales\75.47 - Taller de Desarrollo de Proyectos II\Repositorio\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
     <sheet name="Planificación" sheetId="3" r:id="rId3"/>
     <sheet name="Estado" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -48,9 +53,6 @@
     <t>Exposición</t>
   </si>
   <si>
-    <t>Plan de Respuesta</t>
-  </si>
-  <si>
     <t>Umbral</t>
   </si>
   <si>
@@ -81,9 +83,6 @@
     <t>Si se desarrollase funcionalidad equivocada, se deberá rehacerla, lo que produciría un atraso de cronograma.</t>
   </si>
   <si>
-    <t>Requerimientos</t>
-  </si>
-  <si>
     <t>1) Mala captura de requisitos.      2) Mal análisis de requisitos.</t>
   </si>
   <si>
@@ -114,9 +113,6 @@
     <t>1) Entrega demorada del producto final</t>
   </si>
   <si>
-    <t>Plan de Mitigacion</t>
-  </si>
-  <si>
     <t>Dado que las fechas de exámenes se podrían acumular en un periodo corto de tiempo, se dedicaría una menor cantidad de horas al proyecto en dicho periodo</t>
   </si>
   <si>
@@ -136,13 +132,100 @@
   </si>
   <si>
     <t xml:space="preserve">1) Tecnología nueva                           </t>
+  </si>
+  <si>
+    <t>Es interno</t>
+  </si>
+  <si>
+    <t>Tipo de Riesgo</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Amenaza</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Dado a la tardanza en la comunicación por e-mail por parte del cliente, podría darse el caso que el equipo comience a desarrollar las tareas del nuevo sprint sin confirmación en las prioridades, desarrollando tareas que le resulan poco prioritarias al cliente.</t>
+  </si>
+  <si>
+    <t>Priorización</t>
+  </si>
+  <si>
+    <t>1) Falta de feedback.</t>
+  </si>
+  <si>
+    <t>1) Tareas más prioritarias sin desarrollar.                                2) Mockups no validados</t>
+  </si>
+  <si>
+    <t>Req.</t>
+  </si>
+  <si>
+    <t>Plan de respuesta</t>
+  </si>
+  <si>
+    <t>Mantener una comunicacion constante y fluida con el cliente. Requerir aprobacion de modelos y funcionalidades antes de la entrega misma.</t>
+  </si>
+  <si>
+    <t>Mitigar</t>
+  </si>
+  <si>
+    <t>Ausencia absoluta de comunicacion desde el comienzo de la iteracion hasta la reunion informal.</t>
+  </si>
+  <si>
+    <t>Validar de manera completa modelos y funcionalidades en la reunion informal</t>
+  </si>
+  <si>
+    <t>Llevar un seguimiento de las materias, para mantenerse al dia</t>
+  </si>
+  <si>
+    <t>2 examenes o mas en una misma semana</t>
+  </si>
+  <si>
+    <t>Negociar menor cantidad de user stories para esa iteracion</t>
+  </si>
+  <si>
+    <t>El día de la demo, buscar un laboratorio donde enchufar la computadora a la red de la facultad</t>
+  </si>
+  <si>
+    <t>No conseguir un laboratorio</t>
+  </si>
+  <si>
+    <t>Utilizar datos mocks en el cliente</t>
+  </si>
+  <si>
+    <t>Aclarar requerimientos confusos. Ayudar al cliente a definir el alcance y funcionalidad de los requerimientos</t>
+  </si>
+  <si>
+    <t>Aceptar</t>
+  </si>
+  <si>
+    <t>Informarse y capacitarse en tecnologia dedicada al servicio</t>
+  </si>
+  <si>
+    <t>Retraso de 2 dias respecto a lo estimado</t>
+  </si>
+  <si>
+    <t>Informar sobre el impedimento, e intentar terciarizar el servicio</t>
+  </si>
+  <si>
+    <t>Enviar mails con indicadores de urgencia para obtener una rapida respuesta</t>
+  </si>
+  <si>
+    <t>Llegar al primer sábado después de la primer reunion formal sin el feedback</t>
+  </si>
+  <si>
+    <t>Establecer prioridades de las tareas en la reunion informal, re estimando la cantidad de tareas de ser necesario en base al desarrollo de tareas realizado sin respuesta de prioridades de la primer semana.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,8 +241,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +293,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD7E6B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -487,11 +596,78 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -501,14 +677,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -543,78 +716,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -626,19 +745,186 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -913,7 +1199,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -921,21 +1207,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D2:H24"/>
+  <dimension ref="C2:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="29.5703125" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="10" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
@@ -952,204 +1238,300 @@
     <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="4:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-    </row>
-    <row r="4" spans="4:8" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="3" t="s">
+    <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="29"/>
+    </row>
+    <row r="4" spans="3:10" s="49" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="51" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="4:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D5" s="12">
+      <c r="I4" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="53" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="D5" s="11">
         <v>1</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="H5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="I5" s="58" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="60" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="D6" s="14">
+        <v>2</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="D7" s="14">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="D8" s="14">
+        <v>4</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="F8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="4:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="D6" s="16">
-        <v>2</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="H8" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="D9" s="14">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="4:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D7" s="16">
-        <v>3</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="D8" s="16">
-        <v>4</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="4:8" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="18">
-        <v>5</v>
-      </c>
-      <c r="E9" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="I9" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="61" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="38">
+        <v>6</v>
+      </c>
+      <c r="E10" s="54" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="55" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="54" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="I10" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="J10" s="62" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E14" s="1"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E15" s="1"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E18" s="1"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E19" s="1"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F20" s="2"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="F21" s="2"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="40"/>
+    </row>
+    <row r="15" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="40"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="44"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="40"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="45"/>
+      <c r="H16" s="45"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="40"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="40"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="48"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="40"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="40"/>
+      <c r="D18" s="46"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="40"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="40"/>
+      <c r="D19" s="46"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="40"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="40"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="40"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="40"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="48"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="40"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="40"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D3:H3"/>
+  <mergeCells count="3">
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:J15"/>
+    <mergeCell ref="D3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1158,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E9"/>
+  <dimension ref="B2:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1170,104 +1552,117 @@
     <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="36"/>
+      <c r="B3" s="64" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="66"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="44" t="s">
+      <c r="D4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="45" t="s">
+      <c r="E4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
+      <c r="B5" s="70">
         <v>1</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="71">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="71">
+        <v>0.4</v>
+      </c>
+      <c r="E5" s="72">
         <v>0.2</v>
       </c>
-      <c r="D5" s="22">
-        <v>0.6</v>
-      </c>
-      <c r="E5" s="23">
-        <f>C5*D5</f>
-        <v>0.12</v>
-      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="B6" s="14">
         <v>2</v>
       </c>
-      <c r="C6" s="10">
-        <v>0.8</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="C6" s="63">
         <v>0.7</v>
       </c>
-      <c r="E6" s="24">
-        <f t="shared" ref="E6:E9" si="0">C6*D6</f>
-        <v>0.55999999999999994</v>
+      <c r="D6" s="63">
+        <v>0.2</v>
+      </c>
+      <c r="E6" s="67">
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="10">
-        <v>0.9</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C7" s="63">
         <v>0.5</v>
       </c>
-      <c r="E7" s="24">
-        <f t="shared" si="0"/>
-        <v>0.45</v>
+      <c r="D7" s="63">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="67">
+        <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <v>4</v>
       </c>
-      <c r="C8" s="10">
-        <v>0.6</v>
-      </c>
-      <c r="D8" s="10">
-        <v>0.3</v>
-      </c>
-      <c r="E8" s="24">
-        <f t="shared" si="0"/>
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18">
+      <c r="C8" s="63">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="63">
+        <v>0.2</v>
+      </c>
+      <c r="E8" s="67">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="14">
         <v>5</v>
       </c>
-      <c r="C9" s="25">
+      <c r="C9" s="63">
         <v>0.5</v>
       </c>
-      <c r="D9" s="25">
-        <v>0.4</v>
-      </c>
-      <c r="E9" s="26">
-        <f t="shared" si="0"/>
+      <c r="D9" s="63">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="67">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15">
+        <v>6</v>
+      </c>
+      <c r="C10" s="68">
+        <v>0.7</v>
+      </c>
+      <c r="D10" s="68">
         <v>0.2</v>
+      </c>
+      <c r="E10" s="69">
+        <v>0.14000000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1280,93 +1675,150 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G9"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="39"/>
-    </row>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
+      <c r="B3" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="32"/>
+    </row>
+    <row r="4" spans="2:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="48" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="44" t="s">
+      <c r="C4" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="F4" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="2:7" ht="51" x14ac:dyDescent="0.25">
+      <c r="B5" s="81">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="23"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="C5" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="73" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B6" s="82">
         <v>2</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="24"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="C6" s="79" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="74" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B7" s="82">
         <v>3</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="C7" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" s="74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="B8" s="82">
         <v>4</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="24"/>
-    </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18">
+      <c r="C8" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="56" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="B9" s="82">
         <v>5</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="C9" s="79" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="74" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="83">
+        <v>6</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1378,10 +1830,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F9"/>
+  <dimension ref="B2:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,104 +1847,117 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="35"/>
+    </row>
+    <row r="4" spans="2:6" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="41"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="42"/>
-    </row>
-    <row r="4" spans="2:6" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="44" t="s">
+      <c r="E4" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="F4" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="45" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>1</v>
       </c>
-      <c r="C5" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="22"/>
-      <c r="E5" s="27">
-        <v>41531</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>26</v>
+      <c r="C5" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="16"/>
+      <c r="E5" s="18">
+        <v>41538</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="16">
+      <c r="B6" s="14">
         <v>2</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="47">
-        <v>41531</v>
-      </c>
-      <c r="F6" s="29" t="s">
-        <v>26</v>
+      <c r="C6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="25">
+        <v>41538</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="16">
+      <c r="B7" s="14">
         <v>3</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="47">
-        <v>41531</v>
-      </c>
-      <c r="F7" s="29" t="s">
-        <v>26</v>
+      <c r="C7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="25">
+        <v>41538</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="16">
+      <c r="B8" s="14">
         <v>4</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="47">
-        <v>41531</v>
-      </c>
-      <c r="F8" s="29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="18">
+      <c r="C8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="25">
+        <v>41538</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="84">
         <v>5</v>
       </c>
-      <c r="C9" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="50">
-        <v>41531</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>26</v>
+      <c r="C9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="85"/>
+      <c r="E9" s="25">
+        <v>41538</v>
+      </c>
+      <c r="F9" s="86"/>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="15">
+        <v>6</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="17"/>
+      <c r="E10" s="26">
+        <v>41538</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
# Manejo de Riesgos
</commit_message>
<xml_diff>
--- a/docs/Planilla Registro de Riesgos.xlsx
+++ b/docs/Planilla Registro de Riesgos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>#</t>
   </si>
@@ -219,13 +219,37 @@
   </si>
   <si>
     <t>Establecer prioridades de las tareas en la reunion informal, re estimando la cantidad de tareas de ser necesario en base al desarrollo de tareas realizado sin respuesta de prioridades de la primer semana.</t>
+  </si>
+  <si>
+    <t>Cerrado</t>
+  </si>
+  <si>
+    <t>Dado que no se implementará el servicio de compra con tarjeta de crédito, el riesgo queda cerrado.</t>
+  </si>
+  <si>
+    <t>1) Falta de detalle en la funcionalidad requerida.</t>
+  </si>
+  <si>
+    <t>2) Reportes complejos con poco margen de tiempo para ser realizados</t>
+  </si>
+  <si>
+    <t>Si se demorase la especificación de reportes, se contará con un menor tiempo para realizarlos, lo que generaría un potencial atraso de cronograma de ser reportes complejos</t>
+  </si>
+  <si>
+    <t>Pedir de manera contínua el detalle de especificaciones de cada reporte</t>
+  </si>
+  <si>
+    <t>Llegar al 05/11/2013 sin la especificación de cada reporte</t>
+  </si>
+  <si>
+    <t>Elaborar propuestas de reportes para que el cliente pueda seleccionar de ellas los reportes a realizar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +279,14 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -300,7 +332,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -590,84 +622,6 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -682,60 +636,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -744,51 +662,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -798,67 +671,58 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -869,63 +733,161 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1209,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1220,7 +1182,7 @@
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.28515625" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" style="10" customWidth="1"/>
+    <col min="9" max="9" width="7.5703125" style="4" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
@@ -1240,284 +1202,301 @@
   <sheetData>
     <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="3:10" s="49" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D4" s="50" t="s">
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="31"/>
+    </row>
+    <row r="4" spans="3:10" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="51" t="s">
+      <c r="H4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="52" t="s">
+      <c r="I4" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="53" t="s">
+      <c r="J4" s="85" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="5" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="D5" s="11">
+      <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="58" t="s">
+      <c r="I5" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="60" t="s">
+      <c r="J5" s="22" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" spans="3:10" ht="90" x14ac:dyDescent="0.25">
-      <c r="D6" s="14">
+      <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="81" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="59" t="s">
+      <c r="I6" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="61" t="s">
+      <c r="J6" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="7" spans="3:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="D7" s="14">
+      <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="82" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="81" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="81" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="59" t="s">
+      <c r="I7" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="61" t="s">
+      <c r="J7" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="3:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="D8" s="14">
+      <c r="D8" s="6">
         <v>4</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="81" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="59" t="s">
+      <c r="I8" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J8" s="61" t="s">
+      <c r="J8" s="23" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="3:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="D9" s="14">
+      <c r="D9" s="6">
         <v>5</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="81" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="59" t="s">
+      <c r="I9" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="61" t="s">
+      <c r="J9" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="3:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D10" s="38">
+    <row r="10" spans="3:10" ht="135" x14ac:dyDescent="0.25">
+      <c r="D10" s="86">
         <v>6</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="55" t="s">
+      <c r="F10" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="54" t="s">
+      <c r="G10" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="54" t="s">
+      <c r="H10" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="I10" s="55" t="s">
+      <c r="I10" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="62" t="s">
+      <c r="J10" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="E11" s="1"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+    <row r="11" spans="3:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="46">
+        <v>7</v>
+      </c>
+      <c r="E11" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="83" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="I11" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="24" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E12" s="1"/>
-      <c r="F12" s="6"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="E13" s="1"/>
-      <c r="F13" s="6"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="40"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="11"/>
     </row>
     <row r="15" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="40"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C16" s="40"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="45"/>
-      <c r="H16" s="45"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="40"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="11"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="40"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="47"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="40"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="11"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="40"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="40"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="16"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="40"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="47"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="40"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="11"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="40"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="48"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="40"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="40"/>
-      <c r="D21" s="46"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="57"/>
-      <c r="J21" s="40"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="57"/>
-      <c r="J22" s="40"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="11"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
       <c r="G23" s="1"/>
@@ -1540,10 +1519,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E10"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1560,109 +1539,124 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="66"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="70">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="73">
         <v>0.5</v>
       </c>
-      <c r="D5" s="71">
+      <c r="D5" s="73">
         <v>0.4</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="74">
         <v>0.2</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
+      <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="75">
         <v>0.7</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="75">
         <v>0.2</v>
       </c>
-      <c r="E6" s="67">
+      <c r="E6" s="76">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="14">
+      <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="63">
+      <c r="C7" s="75">
         <v>0.5</v>
       </c>
-      <c r="D7" s="63">
+      <c r="D7" s="75">
         <v>0.05</v>
       </c>
-      <c r="E7" s="67">
+      <c r="E7" s="76">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="14">
+      <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="63">
+      <c r="C8" s="75">
         <v>0.5</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="75">
         <v>0.2</v>
       </c>
-      <c r="E8" s="67">
+      <c r="E8" s="76">
         <v>0.1</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="14">
+      <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="63">
+      <c r="C9" s="75">
         <v>0.5</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="75">
         <v>0.05</v>
       </c>
-      <c r="E9" s="67">
+      <c r="E9" s="76">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="68">
+      <c r="C10" s="75">
         <v>0.7</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D10" s="75">
         <v>0.2</v>
       </c>
-      <c r="E10" s="69">
+      <c r="E10" s="76">
         <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
+        <v>7</v>
+      </c>
+      <c r="C11" s="77">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="77">
+        <v>0.4</v>
+      </c>
+      <c r="E11" s="78">
+        <f>C11*D11</f>
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>
@@ -1675,149 +1669,166 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G10"/>
+  <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="B3" sqref="B3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="3" customWidth="1"/>
     <col min="5" max="5" width="31.42578125" customWidth="1"/>
     <col min="6" max="6" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="32"/>
-    </row>
-    <row r="4" spans="2:7" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="50" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37"/>
+    </row>
+    <row r="4" spans="2:7" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="52" t="s">
+      <c r="D4" s="62" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="53" t="s">
+      <c r="F4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="2:7" ht="51" x14ac:dyDescent="0.25">
-      <c r="B5" s="81">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B5" s="25">
         <v>1</v>
       </c>
-      <c r="C5" s="78" t="s">
+      <c r="C5" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="58" t="s">
+      <c r="D5" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="73" t="s">
+      <c r="F5" s="53" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B6" s="82">
+    <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="26">
         <v>2</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="74" t="s">
+      <c r="F6" s="56" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="82">
+    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B7" s="26">
         <v>3</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="54" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="55" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="74" t="s">
+      <c r="F7" s="56" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="82">
+    <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="26">
         <v>4</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="59" t="s">
+      <c r="D8" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="56" t="s">
+      <c r="E8" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="75" t="s">
+      <c r="F8" s="58" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="82">
+    <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="26">
         <v>5</v>
       </c>
-      <c r="C9" s="79" t="s">
+      <c r="C9" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="74" t="s">
+      <c r="F9" s="56" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="83">
+    <row r="10" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B10" s="26">
         <v>6</v>
       </c>
-      <c r="C10" s="80" t="s">
+      <c r="C10" s="54" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="77" t="s">
+      <c r="D10" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="76" t="s">
+      <c r="F10" s="56" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="48">
+        <v>7</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="49" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="60" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1825,15 +1836,16 @@
     <mergeCell ref="B3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F10"/>
+  <dimension ref="B2:F11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,121 +1854,138 @@
     <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="35"/>
-    </row>
-    <row r="4" spans="2:6" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="22" t="s">
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="40"/>
+    </row>
+    <row r="4" spans="2:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="11">
+      <c r="B5" s="41">
         <v>1</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="16"/>
-      <c r="E5" s="18">
-        <v>41538</v>
-      </c>
-      <c r="F5" s="19" t="s">
+      <c r="D5" s="64"/>
+      <c r="E5" s="65">
+        <v>41570</v>
+      </c>
+      <c r="F5" s="66" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="14">
+      <c r="B6" s="42">
         <v>2</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="25">
-        <v>41538</v>
-      </c>
-      <c r="F6" s="20" t="s">
+      <c r="D6" s="67"/>
+      <c r="E6" s="68">
+        <v>41570</v>
+      </c>
+      <c r="F6" s="69" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="14">
+      <c r="B7" s="42">
         <v>3</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="25">
-        <v>41538</v>
-      </c>
-      <c r="F7" s="20" t="s">
+      <c r="D7" s="67"/>
+      <c r="E7" s="68">
+        <v>41570</v>
+      </c>
+      <c r="F7" s="69" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="14">
+      <c r="B8" s="42">
         <v>4</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="25">
-        <v>41538</v>
-      </c>
-      <c r="F8" s="20" t="s">
+      <c r="D8" s="67"/>
+      <c r="E8" s="68">
+        <v>41570</v>
+      </c>
+      <c r="F8" s="69" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="84">
+    <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="42">
         <v>5</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="67"/>
+      <c r="E9" s="68">
+        <v>41570</v>
+      </c>
+      <c r="F9" s="69" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="42">
+        <v>6</v>
+      </c>
+      <c r="C10" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="85"/>
-      <c r="E9" s="25">
-        <v>41538</v>
-      </c>
-      <c r="F9" s="86"/>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="15">
-        <v>6</v>
-      </c>
-      <c r="C10" s="17" t="s">
+      <c r="D10" s="67"/>
+      <c r="E10" s="68">
+        <v>41570</v>
+      </c>
+      <c r="F10" s="69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="43">
+        <v>7</v>
+      </c>
+      <c r="C11" s="70" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="17"/>
-      <c r="E10" s="26">
-        <v>41538</v>
-      </c>
-      <c r="F10" s="21" t="s">
+      <c r="D11" s="70"/>
+      <c r="E11" s="71">
+        <v>41570</v>
+      </c>
+      <c r="F11" s="72" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated docs for meeting. Item #270
</commit_message>
<xml_diff>
--- a/docs/Planilla Registro de Riesgos.xlsx
+++ b/docs/Planilla Registro de Riesgos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facu\Materias Actuales\75.47 - Taller de Desarrollo de Proyectos II\Repositorio\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian\Documents\UBA\2do Cuat 2013\TallerDesarrollo2\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -86,18 +86,12 @@
     <t>1) Mala captura de requisitos.      2) Mal análisis de requisitos.</t>
   </si>
   <si>
-    <t>1) Retraso de cronograma.           2) Problemas con el cliente.</t>
-  </si>
-  <si>
     <t>Dado que podrían existir cambios constantes de requerimientos, se retrasaría la entrega del producto final.</t>
   </si>
   <si>
     <t>1) Funcionalidad poco clara.          2) Cambios de opinión.</t>
   </si>
   <si>
-    <t>1) Atraso de cronograma.             2) Cambios en el alcance</t>
-  </si>
-  <si>
     <t>Abierto</t>
   </si>
   <si>
@@ -158,9 +152,6 @@
     <t>1) Falta de feedback.</t>
   </si>
   <si>
-    <t>1) Tareas más prioritarias sin desarrollar.                                2) Mockups no validados</t>
-  </si>
-  <si>
     <t>Req.</t>
   </si>
   <si>
@@ -215,9 +206,6 @@
     <t>Enviar mails con indicadores de urgencia para obtener una rapida respuesta</t>
   </si>
   <si>
-    <t>Llegar al primer sábado después de la primer reunion formal sin el feedback</t>
-  </si>
-  <si>
     <t>Establecer prioridades de las tareas en la reunion informal, re estimando la cantidad de tareas de ser necesario en base al desarrollo de tareas realizado sin respuesta de prioridades de la primer semana.</t>
   </si>
   <si>
@@ -230,9 +218,6 @@
     <t>1) Falta de detalle en la funcionalidad requerida.</t>
   </si>
   <si>
-    <t>2) Reportes complejos con poco margen de tiempo para ser realizados</t>
-  </si>
-  <si>
     <t>Si se demorase la especificación de reportes, se contará con un menor tiempo para realizarlos, lo que generaría un potencial atraso de cronograma de ser reportes complejos</t>
   </si>
   <si>
@@ -243,6 +228,24 @@
   </si>
   <si>
     <t>Elaborar propuestas de reportes para que el cliente pueda seleccionar de ellas los reportes a realizar</t>
+  </si>
+  <si>
+    <t>Terminar el primer sábado después de la primer reunion formal sin el feedback</t>
+  </si>
+  <si>
+    <t>1) Retraso de cronograma. 
+2) Problemas con el cliente.</t>
+  </si>
+  <si>
+    <t>1) Atraso de cronograma. 
+2) Cambios en el alcance</t>
+  </si>
+  <si>
+    <t>1) Tareas más prioritarias sin desarrollar.
+2) Mockups no validados</t>
+  </si>
+  <si>
+    <t>1) Menor cantidad de reportes podrán ser realizados</t>
   </si>
 </sst>
 </file>
@@ -709,6 +712,144 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -750,144 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1171,17 +1174,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C3" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.140625" customWidth="1"/>
+    <col min="5" max="5" width="81.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="7" max="7" width="40.140625" customWidth="1"/>
+    <col min="8" max="8" width="34" customWidth="1"/>
     <col min="9" max="9" width="7.5703125" style="4" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" customWidth="1"/>
     <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -1202,15 +1205,15 @@
   <sheetData>
     <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="31"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="77"/>
     </row>
     <row r="4" spans="3:10" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D4" s="19" t="s">
@@ -1228,172 +1231,172 @@
       <c r="H4" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="84" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="85" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="I4" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="71" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="79" t="s">
+      <c r="E5" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="80" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="79" t="s">
+      <c r="F5" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="79" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="51" t="s">
-        <v>37</v>
+      <c r="H5" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>35</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="3:10" ht="90" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" ht="60" x14ac:dyDescent="0.25">
       <c r="D6" s="6">
         <v>2</v>
       </c>
-      <c r="E6" s="81" t="s">
+      <c r="E6" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="81" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="81" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" s="45" t="s">
-        <v>39</v>
+      <c r="I6" s="31" t="s">
+        <v>37</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" ht="45" x14ac:dyDescent="0.25">
       <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="E7" s="81" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="82" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="81" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="81" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="45" t="s">
-        <v>37</v>
+      <c r="E7" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="67" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="31" t="s">
+        <v>35</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="3:10" ht="60" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D8" s="6">
         <v>4</v>
       </c>
-      <c r="E8" s="81" t="s">
+      <c r="E8" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="82" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="81" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="45" t="s">
-        <v>37</v>
+      <c r="H8" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" s="31" t="s">
+        <v>35</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="3:10" ht="75" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="3:10" ht="30" x14ac:dyDescent="0.25">
       <c r="D9" s="6">
         <v>5</v>
       </c>
-      <c r="E9" s="81" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="82" t="s">
-        <v>44</v>
-      </c>
-      <c r="G9" s="81" t="s">
-        <v>34</v>
-      </c>
-      <c r="H9" s="81" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="45" t="s">
+      <c r="E9" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="68" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="I9" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="D10" s="72">
+        <v>6</v>
+      </c>
+      <c r="E10" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="3:10" ht="135" x14ac:dyDescent="0.25">
-      <c r="D10" s="86">
-        <v>6</v>
-      </c>
-      <c r="E10" s="44" t="s">
+      <c r="G10" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="H10" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="J10" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="32">
+        <v>7</v>
+      </c>
+      <c r="E11" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="I10" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="J10" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="3:10" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D11" s="46">
-        <v>7</v>
-      </c>
-      <c r="E11" s="83" t="s">
-        <v>68</v>
-      </c>
-      <c r="F11" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="83" t="s">
-        <v>66</v>
-      </c>
-      <c r="H11" s="83" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="49" t="s">
-        <v>37</v>
+      <c r="G11" s="69" t="s">
+        <v>62</v>
+      </c>
+      <c r="H11" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.25">
@@ -1420,17 +1423,17 @@
     </row>
     <row r="15" spans="3:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="11"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="74"/>
+      <c r="G15" s="74"/>
+      <c r="H15" s="74"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="11"/>
-      <c r="D16" s="27"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="14"/>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1539,12 +1542,12 @@
   <sheetData>
     <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="34"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="80"/>
     </row>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
@@ -1564,13 +1567,13 @@
       <c r="B5" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="73">
+      <c r="C5" s="59">
         <v>0.5</v>
       </c>
-      <c r="D5" s="73">
+      <c r="D5" s="59">
         <v>0.4</v>
       </c>
-      <c r="E5" s="74">
+      <c r="E5" s="60">
         <v>0.2</v>
       </c>
     </row>
@@ -1578,13 +1581,13 @@
       <c r="B6" s="6">
         <v>2</v>
       </c>
-      <c r="C6" s="75">
+      <c r="C6" s="61">
         <v>0.7</v>
       </c>
-      <c r="D6" s="75">
+      <c r="D6" s="61">
         <v>0.2</v>
       </c>
-      <c r="E6" s="76">
+      <c r="E6" s="62">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -1592,13 +1595,13 @@
       <c r="B7" s="6">
         <v>3</v>
       </c>
-      <c r="C7" s="75">
+      <c r="C7" s="61">
         <v>0.5</v>
       </c>
-      <c r="D7" s="75">
+      <c r="D7" s="61">
         <v>0.05</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="62">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -1606,13 +1609,13 @@
       <c r="B8" s="6">
         <v>4</v>
       </c>
-      <c r="C8" s="75">
+      <c r="C8" s="61">
         <v>0.5</v>
       </c>
-      <c r="D8" s="75">
+      <c r="D8" s="61">
         <v>0.2</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="62">
         <v>0.1</v>
       </c>
     </row>
@@ -1620,13 +1623,13 @@
       <c r="B9" s="6">
         <v>5</v>
       </c>
-      <c r="C9" s="75">
+      <c r="C9" s="61">
         <v>0.5</v>
       </c>
-      <c r="D9" s="75">
+      <c r="D9" s="61">
         <v>0.05</v>
       </c>
-      <c r="E9" s="76">
+      <c r="E9" s="62">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
@@ -1634,13 +1637,13 @@
       <c r="B10" s="6">
         <v>6</v>
       </c>
-      <c r="C10" s="75">
+      <c r="C10" s="61">
         <v>0.7</v>
       </c>
-      <c r="D10" s="75">
+      <c r="D10" s="61">
         <v>0.2</v>
       </c>
-      <c r="E10" s="76">
+      <c r="E10" s="62">
         <v>0.14000000000000001</v>
       </c>
     </row>
@@ -1648,13 +1651,13 @@
       <c r="B11" s="7">
         <v>7</v>
       </c>
-      <c r="C11" s="77">
+      <c r="C11" s="63">
         <v>0.5</v>
       </c>
-      <c r="D11" s="77">
+      <c r="D11" s="63">
         <v>0.4</v>
       </c>
-      <c r="E11" s="78">
+      <c r="E11" s="64">
         <f>C11*D11</f>
         <v>0.2</v>
       </c>
@@ -1672,7 +1675,7 @@
   <dimension ref="B2:G11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:F3"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1686,28 +1689,28 @@
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="81" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="37"/>
+      <c r="C3" s="82"/>
+      <c r="D3" s="82"/>
+      <c r="E3" s="82"/>
+      <c r="F3" s="83"/>
     </row>
     <row r="4" spans="2:7" s="3" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="47" t="s">
+      <c r="B4" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="62" t="s">
+      <c r="C4" s="48" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="62" t="s">
+      <c r="E4" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="63" t="s">
+      <c r="F4" s="49" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="2"/>
@@ -1716,119 +1719,119 @@
       <c r="B5" s="25">
         <v>1</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="39" t="s">
         <v>46</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="53" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="26">
         <v>2</v>
       </c>
-      <c r="C6" s="54" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" s="45" t="s">
+      <c r="C6" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="55" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="56" t="s">
-        <v>52</v>
+      <c r="D6" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="26">
         <v>3</v>
       </c>
-      <c r="C7" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="55" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="56" t="s">
-        <v>55</v>
+      <c r="C7" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" s="26">
         <v>4</v>
       </c>
-      <c r="C8" s="54" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="57" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="58" t="s">
-        <v>24</v>
+      <c r="C8" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="43" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="26">
         <v>5</v>
       </c>
-      <c r="C9" s="54" t="s">
-        <v>58</v>
-      </c>
-      <c r="D9" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="56" t="s">
-        <v>60</v>
+      <c r="C9" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="42" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B10" s="26">
         <v>6</v>
       </c>
-      <c r="C10" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="45" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="55" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="56" t="s">
-        <v>63</v>
+      <c r="C10" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="48">
+      <c r="B11" s="34">
         <v>7</v>
       </c>
-      <c r="C11" s="59" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="49" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="60" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" s="61" t="s">
-        <v>71</v>
+      <c r="C11" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="47" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1859,13 +1862,13 @@
   <sheetData>
     <row r="2" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="84" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="40"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="86"/>
     </row>
     <row r="4" spans="2:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
@@ -1885,108 +1888,108 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="41">
+      <c r="B5" s="27">
         <v>1</v>
       </c>
-      <c r="C5" s="64" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65">
+      <c r="C5" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="50"/>
+      <c r="E5" s="51">
         <v>41570</v>
       </c>
-      <c r="F5" s="66" t="s">
-        <v>24</v>
+      <c r="F5" s="52" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="42">
+      <c r="B6" s="28">
         <v>2</v>
       </c>
-      <c r="C6" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="67"/>
-      <c r="E6" s="68">
+      <c r="C6" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54">
         <v>41570</v>
       </c>
-      <c r="F6" s="69" t="s">
-        <v>24</v>
+      <c r="F6" s="55" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="42">
+      <c r="B7" s="28">
         <v>3</v>
       </c>
-      <c r="C7" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="67"/>
-      <c r="E7" s="68">
+      <c r="C7" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="53"/>
+      <c r="E7" s="54">
         <v>41570</v>
       </c>
-      <c r="F7" s="69" t="s">
-        <v>24</v>
+      <c r="F7" s="55" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="42">
+      <c r="B8" s="28">
         <v>4</v>
       </c>
-      <c r="C8" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="67"/>
-      <c r="E8" s="68">
+      <c r="C8" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="53"/>
+      <c r="E8" s="54">
         <v>41570</v>
       </c>
-      <c r="F8" s="69" t="s">
-        <v>24</v>
+      <c r="F8" s="55" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="42">
+      <c r="B9" s="28">
         <v>5</v>
       </c>
-      <c r="C9" s="67" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="67"/>
-      <c r="E9" s="68">
+      <c r="C9" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="D9" s="53"/>
+      <c r="E9" s="54">
         <v>41570</v>
       </c>
-      <c r="F9" s="69" t="s">
-        <v>65</v>
+      <c r="F9" s="55" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="42">
+      <c r="B10" s="28">
         <v>6</v>
       </c>
-      <c r="C10" s="67" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="67"/>
-      <c r="E10" s="68">
+      <c r="C10" s="53" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="53"/>
+      <c r="E10" s="54">
         <v>41570</v>
       </c>
-      <c r="F10" s="69" t="s">
-        <v>24</v>
+      <c r="F10" s="55" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="43">
+      <c r="B11" s="29">
         <v>7</v>
       </c>
-      <c r="C11" s="70" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="70"/>
-      <c r="E11" s="71">
+      <c r="C11" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57">
         <v>41570</v>
       </c>
-      <c r="F11" s="72" t="s">
-        <v>24</v>
+      <c r="F11" s="58" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>